<commit_message>
- project for generating sql templates
</commit_message>
<xml_diff>
--- a/db/categories.xlsx
+++ b/db/categories.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\Desktop\UFO\Assets\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Git Repositories\Github\FH-Hagenberg\SemesterProject1516\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32400" windowHeight="18615"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>